<commit_message>
Add answer decoding to review the ones incorrectly predicted.
Update excel to show incorrectly predicted text answers.
</commit_message>
<xml_diff>
--- a/data/Results/SciEntsData Hypertuning.xlsx
+++ b/data/Results/SciEntsData Hypertuning.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbrandt/Dropbox/PycharmProjects/short_answer_granding_capstone_project/data/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13811D25-07FF-2B4A-9430-CA7879AF03EE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714FE089-9DEF-E949-987A-71B7BFCFCF02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20040" yWindow="2700" windowWidth="28040" windowHeight="17440" xr2:uid="{74EE537B-979F-D844-81CC-929D075ED3E5}"/>
+    <workbookView xWindow="20040" yWindow="2700" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{74EE537B-979F-D844-81CC-929D075ED3E5}"/>
   </bookViews>
   <sheets>
     <sheet name="SciEntsData Hypertuning Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="83">
   <si>
     <t>Validation_loss</t>
   </si>
@@ -124,19 +126,181 @@
   </si>
   <si>
     <t>sagemaker-tensorflow-190625-2206-018-d8056d1e/algo-1-1561501194</t>
+  </si>
+  <si>
+    <t>raw_predicted</t>
+  </si>
+  <si>
+    <t>predicted</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.0 answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the nickel is the hardest becaus is you scratch it with a penni it will not scratch but the nickel could becaus it is so much</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.0 answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> becaus a solut is clear but other mixtur are not</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the magnet do not touch becaus if you flip the magnet to the other side it will not stick becaus it make them differ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> it is one materi that dissolv into the other make a clear mixtur although it could be color it ha to be see through</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> which had less scratch</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> it is a clear mixtur</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> by use your hand</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> how you would know that one of them is harder is for say if the nickel never a scratch the penni and the penni got scratch by the nickel then the nickel would be harder than the penni that is how you would which one is harder</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> they are not touch each other becaus they repel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the one that is harder will scratch the less harder one</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> they are repel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the ring do not touch each other becaus if the magnet are not the right way they will repel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the magnet are not touch becaus the magnet forc is make the magnet repel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> when the string is tighten the pitch is higher not lower</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> when it wa loos the sound wa soft but when it wa tighten it is low</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the string wa higher pitch becaus it had more tension</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the ring do not touch becaus the ring are just magnet and the magnet are on the repel side</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> when you make it long it make it low sound when you make it short it a height sound</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> in order to tell which is harder els would have to see if the penni and nickel leav a mark to see which is harder</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the nickel is the heavier and the penni is the lighter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> they do not touch each other becaus if you put magnet the magnet like thi will not attract north to north if you put magnet like thi it will attract north to south if you put it like thi it will not attract south to south</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> she would know becaus the one that is scratch is the one that is least hard and the one that is not scratch is the one that is hardest</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> they are on the same side</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> it would make a high sound</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> she could tell which is harder by get a rock and see if the penni or nickel would scratch it whichev one doe is harder</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> she would scratch the rock togeth the one that scratch is softer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> it dissolv the solid into a liquid that is see through</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the magnet are not touch becaus they are flip around a certain way that they do not stick instead they repel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the one that is scratch is softer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> it ha to be a fairli clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the string is lower when you tighten it</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the ring do not touch becaus the top is south pole is the one below it is the south pole when the pole are north and south they attract</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> a solut is differ becaus a solut is a mixtur of a solid materi and a liquid</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mayb he should scratch even other then when you are done see if one have scratch</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> clear and thing that make it still clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> i do not know</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> it wa soft then it got louder</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> a solut is when you take a mixtur like powder and mix it with water then after stir it it becom a solut</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> becaus of it he you scratch with a penni</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> a solut doe not dissolv</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> in a solut one of the materi dissolv and the mixtur is see through</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the magnet will mayb not stick becaus the forc of the magnet will mayb the pencil is long and the magnet cannot feel the other magnet</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> correct</t>
+  </si>
+  <si>
+    <t>The harder coin will scratch the other</t>
+  </si>
+  <si>
+    <t>When the string was tighter, the pitch was higher.</t>
+  </si>
+  <si>
+    <t>A solution is a mixture formed when a solid dissolves in a liquid.</t>
+  </si>
+  <si>
+    <t>Like poles repel and opposite poles attract.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,8 +323,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4187893-C62D-BB41-AE0E-B9FEF22E5CB0}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -1069,4 +1237,982 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A651DD34-854C-7143-8D50-B2457B0FF092}">
+  <dimension ref="A1:K43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="101.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="49" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-6.3559999999999997E-3</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f>VLOOKUP(A2,G$2:K$43,5,FALSE)</f>
+        <v xml:space="preserve"> the nickel is the hardest becaus is you scratch it with a penni it will not scratch but the nickel could becaus it is so much</v>
+      </c>
+      <c r="F2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G2">
+        <f>H2+1</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0.46917399999999998</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f t="shared" ref="E3:E11" si="0">VLOOKUP(A3,G$2:K$43,5,FALSE)</f>
+        <v xml:space="preserve"> which had less scratch</v>
+      </c>
+      <c r="F3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G43" si="1">H3+1</f>
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>-0.26127</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> how you would know that one of them is harder is for say if the nickel never a scratch the penni and the penni got scratch by the nickel then the nickel would be harder than the penni that is how you would which one is harder</v>
+      </c>
+      <c r="F4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>78</v>
+      </c>
+      <c r="J4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>0.97733999999999999</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> when it wa loos the sound wa soft but when it wa tighten it is low</v>
+      </c>
+      <c r="F5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>0.98013499999999998</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> the ring do not touch becaus the ring are just magnet and the magnet are on the repel side</v>
+      </c>
+      <c r="F6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>-6.7739999999999996E-3</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> in order to tell which is harder els would have to see if the penni and nickel leav a mark to see which is harder</v>
+      </c>
+      <c r="F7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>-0.12531300000000001</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> they do not touch each other becaus if you put magnet the magnet like thi will not attract north to north if you put magnet like thi it will attract north to south if you put it like thi it will not attract south to south</v>
+      </c>
+      <c r="F8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J8" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>0.16872599999999999</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> it would make a high sound</v>
+      </c>
+      <c r="F9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9" t="s">
+        <v>78</v>
+      </c>
+      <c r="J9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>-1.9989999999999999E-3</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> a solut is when you take a mixtur like powder and mix it with water then after stir it it becom a solut</v>
+      </c>
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>41</v>
+      </c>
+      <c r="B11">
+        <v>2.7300000000000002E-4</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> in a solut one of the materi dissolv and the mixtur is see through</v>
+      </c>
+      <c r="F11" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>9</v>
+      </c>
+      <c r="I11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
+      <c r="I13" t="s">
+        <v>78</v>
+      </c>
+      <c r="J13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
+      <c r="I14" t="s">
+        <v>78</v>
+      </c>
+      <c r="J14" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="H15">
+        <v>13</v>
+      </c>
+      <c r="I15" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>14</v>
+      </c>
+      <c r="I16" t="s">
+        <v>78</v>
+      </c>
+      <c r="J16" t="s">
+        <v>36</v>
+      </c>
+      <c r="K16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="H17">
+        <v>15</v>
+      </c>
+      <c r="I17" t="s">
+        <v>78</v>
+      </c>
+      <c r="J17" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="H18">
+        <v>16</v>
+      </c>
+      <c r="I18" t="s">
+        <v>78</v>
+      </c>
+      <c r="J18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="H19">
+        <v>17</v>
+      </c>
+      <c r="I19" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="H20">
+        <v>18</v>
+      </c>
+      <c r="I20" t="s">
+        <v>78</v>
+      </c>
+      <c r="J20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="H21">
+        <v>19</v>
+      </c>
+      <c r="I21" t="s">
+        <v>78</v>
+      </c>
+      <c r="J21" t="s">
+        <v>36</v>
+      </c>
+      <c r="K21" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="H22">
+        <v>20</v>
+      </c>
+      <c r="I22" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="H23">
+        <v>21</v>
+      </c>
+      <c r="I23" t="s">
+        <v>78</v>
+      </c>
+      <c r="J23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="H24">
+        <v>22</v>
+      </c>
+      <c r="I24" t="s">
+        <v>78</v>
+      </c>
+      <c r="J24" t="s">
+        <v>36</v>
+      </c>
+      <c r="K24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="H25">
+        <v>23</v>
+      </c>
+      <c r="I25" t="s">
+        <v>78</v>
+      </c>
+      <c r="J25" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="H26">
+        <v>24</v>
+      </c>
+      <c r="I26" t="s">
+        <v>78</v>
+      </c>
+      <c r="J26" t="s">
+        <v>36</v>
+      </c>
+      <c r="K26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="H27">
+        <v>25</v>
+      </c>
+      <c r="I27" t="s">
+        <v>78</v>
+      </c>
+      <c r="J27" t="s">
+        <v>34</v>
+      </c>
+      <c r="K27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="H28">
+        <v>26</v>
+      </c>
+      <c r="I28" t="s">
+        <v>78</v>
+      </c>
+      <c r="J28" t="s">
+        <v>34</v>
+      </c>
+      <c r="K28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="H29">
+        <v>27</v>
+      </c>
+      <c r="I29" t="s">
+        <v>78</v>
+      </c>
+      <c r="J29" t="s">
+        <v>36</v>
+      </c>
+      <c r="K29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="H30">
+        <v>28</v>
+      </c>
+      <c r="I30" t="s">
+        <v>78</v>
+      </c>
+      <c r="J30" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="H31">
+        <v>29</v>
+      </c>
+      <c r="I31" t="s">
+        <v>78</v>
+      </c>
+      <c r="J31" t="s">
+        <v>36</v>
+      </c>
+      <c r="K31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="H32">
+        <v>30</v>
+      </c>
+      <c r="I32" t="s">
+        <v>78</v>
+      </c>
+      <c r="J32" t="s">
+        <v>36</v>
+      </c>
+      <c r="K32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="H33">
+        <v>31</v>
+      </c>
+      <c r="I33" t="s">
+        <v>78</v>
+      </c>
+      <c r="J33" t="s">
+        <v>34</v>
+      </c>
+      <c r="K33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="H34">
+        <v>32</v>
+      </c>
+      <c r="I34" t="s">
+        <v>78</v>
+      </c>
+      <c r="J34" t="s">
+        <v>36</v>
+      </c>
+      <c r="K34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="H35">
+        <v>33</v>
+      </c>
+      <c r="I35" t="s">
+        <v>78</v>
+      </c>
+      <c r="J35" t="s">
+        <v>36</v>
+      </c>
+      <c r="K35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="H36">
+        <v>34</v>
+      </c>
+      <c r="I36" t="s">
+        <v>78</v>
+      </c>
+      <c r="J36" t="s">
+        <v>36</v>
+      </c>
+      <c r="K36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="H37">
+        <v>35</v>
+      </c>
+      <c r="I37" t="s">
+        <v>78</v>
+      </c>
+      <c r="J37" t="s">
+        <v>36</v>
+      </c>
+      <c r="K37" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="H38">
+        <v>36</v>
+      </c>
+      <c r="I38" t="s">
+        <v>78</v>
+      </c>
+      <c r="J38" t="s">
+        <v>36</v>
+      </c>
+      <c r="K38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="H39">
+        <v>37</v>
+      </c>
+      <c r="I39" t="s">
+        <v>78</v>
+      </c>
+      <c r="J39" t="s">
+        <v>34</v>
+      </c>
+      <c r="K39" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="H40">
+        <v>38</v>
+      </c>
+      <c r="I40" t="s">
+        <v>78</v>
+      </c>
+      <c r="J40" t="s">
+        <v>36</v>
+      </c>
+      <c r="K40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="H41">
+        <v>39</v>
+      </c>
+      <c r="I41" t="s">
+        <v>78</v>
+      </c>
+      <c r="J41" t="s">
+        <v>36</v>
+      </c>
+      <c r="K41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="H42">
+        <v>40</v>
+      </c>
+      <c r="I42" t="s">
+        <v>78</v>
+      </c>
+      <c r="J42" t="s">
+        <v>34</v>
+      </c>
+      <c r="K42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="7:11" x14ac:dyDescent="0.2">
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="H43">
+        <v>41</v>
+      </c>
+      <c r="I43" t="s">
+        <v>78</v>
+      </c>
+      <c r="J43" t="s">
+        <v>36</v>
+      </c>
+      <c r="K43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Clean up Spreadsheet of SciEntsBank results
</commit_message>
<xml_diff>
--- a/data/Results/SciEntsData Hypertuning.xlsx
+++ b/data/Results/SciEntsData Hypertuning.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbrandt/Dropbox/PycharmProjects/short_answer_granding_capstone_project/data/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{714FE089-9DEF-E949-987A-71B7BFCFCF02}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C74B975-6273-AB4F-BEDB-A46EE9742092}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20040" yWindow="2700" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{74EE537B-979F-D844-81CC-929D075ED3E5}"/>
+    <workbookView xWindow="24840" yWindow="2220" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{74EE537B-979F-D844-81CC-929D075ED3E5}"/>
   </bookViews>
   <sheets>
     <sheet name="SciEntsData Hypertuning Results" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Source Sentences" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1243,14 +1242,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A651DD34-854C-7143-8D50-B2457B0FF092}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="5" max="5" width="101.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="124" style="2" customWidth="1"/>
     <col min="6" max="6" width="49" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Update Spreadsheats for Hypertuning results data
</commit_message>
<xml_diff>
--- a/data/Results/SciEntsData Hypertuning.xlsx
+++ b/data/Results/SciEntsData Hypertuning.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbrandt/Dropbox/PycharmProjects/short_answer_granding_capstone_project/data/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C74B975-6273-AB4F-BEDB-A46EE9742092}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1063DEF-2AA8-9041-8063-2785BC24D3BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24840" yWindow="2220" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{74EE537B-979F-D844-81CC-929D075ED3E5}"/>
+    <workbookView xWindow="26220" yWindow="1400" windowWidth="28040" windowHeight="17440" xr2:uid="{74EE537B-979F-D844-81CC-929D075ED3E5}"/>
   </bookViews>
   <sheets>
     <sheet name="SciEntsData Hypertuning Results" sheetId="1" r:id="rId1"/>
     <sheet name="Source Sentences" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -287,7 +290,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -300,6 +307,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -319,18 +333,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -343,6 +361,3369 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SciEntsData Hypertuning Results'!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>dropout</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'SciEntsData Hypertuning Results'!$A$2:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0.38547532152095398</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22199686351997999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.20300461839595399</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.38364195774972998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.44596580996139501</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.23362639056012</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.36786325122251501</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.39112717698970401</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.223719950427204</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.37640549730220402</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.35601975511470402</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.20300461839595399</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.39577169558249597</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.233829325427204</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.20838181566157901</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.38423630784907897</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.24786251961875</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.42492890731560701</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.219713846911579</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.36497541610466999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.35909773055779498</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.47818073837029501</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>0.32545903287280598</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'SciEntsData Hypertuning Results'!$F$2:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0.76744186600973396</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76744185907896101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74418605205624599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.72093023810275703</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.72093023117198496</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.72093023117198496</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.72093023117198496</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.72093023117198496</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.69767441721849599</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.69767441721849599</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.69767441721849599</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.69767441721849599</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.67441860326500802</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.65116278931151905</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.65116278931151905</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.60465116833531496</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.60465116833531496</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.60465116833531496</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.60465116001838803</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D3FF-D043-A4B7-EB536971E742}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1763048527"/>
+        <c:axId val="1763050159"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1763048527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1763050159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1763050159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1763048527"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SciEntsData Hypertuning Results'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>embedding_size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'SciEntsData Hypertuning Results'!$B$2:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'SciEntsData Hypertuning Results'!$F$2:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0.76744186600973396</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76744185907896101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74418605205624599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.72093023810275703</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.72093023117198496</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.72093023117198496</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.72093023117198496</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.72093023117198496</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.69767441721849599</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.69767441721849599</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.69767441721849599</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.69767441721849599</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.67441860326500802</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.65116278931151905</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.65116278931151905</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.60465116833531496</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.60465116833531496</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.60465116833531496</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.60465116001838803</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ACAF-4142-97E1-8314A7284E63}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1763048527"/>
+        <c:axId val="1763050159"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1763048527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1763050159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1763050159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1763048527"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SciEntsData Hypertuning Results'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>lstm_size</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'SciEntsData Hypertuning Results'!$D$2:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>147</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>138</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'SciEntsData Hypertuning Results'!$F$2:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>0.0%</c:formatCode>
+                <c:ptCount val="24"/>
+                <c:pt idx="0">
+                  <c:v>0.76744186600973396</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.76744185907896101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.74418605205624599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.74418604512547304</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.72093023810275703</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.72093023117198496</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.72093023117198496</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.72093023117198496</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.72093023117198496</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.69767441721849599</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.69767441721849599</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.69767441721849599</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.69767441721849599</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.67441860326500802</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.65116278931151905</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.65116278931151905</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.60465116833531496</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.60465116833531496</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.60465116833531496</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.60465116001838803</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9130-BD4A-A91C-AE76EF471BCC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1763048527"/>
+        <c:axId val="1763050159"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1763048527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1763050159"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1763050159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1763048527"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E20A4DB8-84E2-264C-9BE6-E2C6E999F27A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>863600</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{773284F7-27F4-2C44-9CCC-F1CA831EF760}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F9EF56E-E2AF-1341-93DF-3DB80DA15D65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="ShortAnswer Hypertuning Results"/>
+      <sheetName val="Source Sentences"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="A2">
+            <v>0.38547532152095398</v>
+          </cell>
+          <cell r="F2">
+            <v>0.76744186600973396</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>0.22199686351997999</v>
+          </cell>
+          <cell r="F3">
+            <v>0.76744185907896101</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>0.20300461839595399</v>
+          </cell>
+          <cell r="F4">
+            <v>0.74418605205624599</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>0.38364195774972998</v>
+          </cell>
+          <cell r="F5">
+            <v>0.74418604512547304</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>0.44596580996139501</v>
+          </cell>
+          <cell r="F6">
+            <v>0.74418604512547304</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>0.23362639056012</v>
+          </cell>
+          <cell r="F7">
+            <v>0.74418604512547304</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>0.36786325122251501</v>
+          </cell>
+          <cell r="F8">
+            <v>0.74418604512547304</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>0.39112717698970401</v>
+          </cell>
+          <cell r="F9">
+            <v>0.74418604512547304</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>0.223719950427204</v>
+          </cell>
+          <cell r="F10">
+            <v>0.72093023810275703</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>0.37640549730220402</v>
+          </cell>
+          <cell r="F11">
+            <v>0.72093023117198496</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>0.35601975511470402</v>
+          </cell>
+          <cell r="F12">
+            <v>0.72093023117198496</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>0.20300461839595399</v>
+          </cell>
+          <cell r="F13">
+            <v>0.72093023117198496</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>0.39577169558249597</v>
+          </cell>
+          <cell r="F14">
+            <v>0.72093023117198496</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>0.233829325427204</v>
+          </cell>
+          <cell r="F15">
+            <v>0.69767441721849599</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>0.20838181566157901</v>
+          </cell>
+          <cell r="F16">
+            <v>0.69767441721849599</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>0.2</v>
+          </cell>
+          <cell r="F17">
+            <v>0.69767441721849599</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>0.38423630784907897</v>
+          </cell>
+          <cell r="F18">
+            <v>0.69767441721849599</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>0.24786251961875</v>
+          </cell>
+          <cell r="F19">
+            <v>0.67441860326500802</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>0.42492890731560701</v>
+          </cell>
+          <cell r="F20">
+            <v>0.65116278931151905</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>0.219713846911579</v>
+          </cell>
+          <cell r="F21">
+            <v>0.65116278931151905</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>0.36497541610466999</v>
+          </cell>
+          <cell r="F22">
+            <v>0.60465116833531496</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>0.35909773055779498</v>
+          </cell>
+          <cell r="F23">
+            <v>0.60465116833531496</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>0.47818073837029501</v>
+          </cell>
+          <cell r="F24">
+            <v>0.60465116833531496</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>0.32545903287280598</v>
+          </cell>
+          <cell r="F25">
+            <v>0.60465116001838803</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -644,8 +4025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4187893-C62D-BB41-AE0E-B9FEF22E5CB0}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -679,7 +4060,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>0.38547532152095398</v>
       </c>
       <c r="B2">
@@ -691,10 +4072,10 @@
       <c r="D2">
         <v>147</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>0.255741164434787</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>0.76744186600973396</v>
       </c>
       <c r="G2" t="s">
@@ -702,7 +4083,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>0.22199686351997999</v>
       </c>
       <c r="B3">
@@ -714,10 +4095,10 @@
       <c r="D3">
         <v>97</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>0.24057497915833401</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>0.76744185907896101</v>
       </c>
       <c r="G3" t="s">
@@ -725,7 +4106,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>0.20300461839595399</v>
       </c>
       <c r="B4">
@@ -737,10 +4118,10 @@
       <c r="D4">
         <v>118</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>0.26060245480648297</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>0.74418605205624599</v>
       </c>
       <c r="G4" t="s">
@@ -748,7 +4129,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>0.38364195774972998</v>
       </c>
       <c r="B5">
@@ -760,10 +4141,10 @@
       <c r="D5">
         <v>179</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>0.27446782138458498</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>0.74418604512547304</v>
       </c>
       <c r="G5" t="s">
@@ -771,7 +4152,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>0.44596580996139501</v>
       </c>
       <c r="B6">
@@ -783,10 +4164,10 @@
       <c r="D6">
         <v>83</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>0.24562144314133799</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>0.74418604512547304</v>
       </c>
       <c r="G6" t="s">
@@ -794,7 +4175,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>0.23362639056012</v>
       </c>
       <c r="B7">
@@ -806,10 +4187,10 @@
       <c r="D7">
         <v>107</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>0.24299895936666499</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>0.74418604512547304</v>
       </c>
       <c r="G7" t="s">
@@ -817,7 +4198,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>0.36786325122251501</v>
       </c>
       <c r="B8">
@@ -829,10 +4210,10 @@
       <c r="D8">
         <v>124</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <v>0.24509148403655601</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>0.74418604512547304</v>
       </c>
       <c r="G8" t="s">
@@ -840,7 +4221,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>0.39112717698970401</v>
       </c>
       <c r="B9">
@@ -852,10 +4233,10 @@
       <c r="D9">
         <v>93</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>0.279094595202179</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="3">
         <v>0.74418604512547304</v>
       </c>
       <c r="G9" t="s">
@@ -863,7 +4244,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>0.223719950427204</v>
       </c>
       <c r="B10">
@@ -875,10 +4256,10 @@
       <c r="D10">
         <v>88</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <v>0.28327261050080099</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>0.72093023810275703</v>
       </c>
       <c r="G10" t="s">
@@ -886,7 +4267,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>0.37640549730220402</v>
       </c>
       <c r="B11">
@@ -898,10 +4279,10 @@
       <c r="D11">
         <v>133</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <v>0.30613542053588599</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="3">
         <v>0.72093023117198496</v>
       </c>
       <c r="G11" t="s">
@@ -909,7 +4290,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="4">
         <v>0.35601975511470402</v>
       </c>
       <c r="B12">
@@ -921,10 +4302,10 @@
       <c r="D12">
         <v>108</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <v>0.27214143373245397</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>0.72093023117198496</v>
       </c>
       <c r="G12" t="s">
@@ -932,7 +4313,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="4">
         <v>0.20300461839595399</v>
       </c>
       <c r="B13">
@@ -944,10 +4325,10 @@
       <c r="D13">
         <v>119</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <v>0.27320282785005301</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>0.72093023117198496</v>
       </c>
       <c r="G13" t="s">
@@ -955,7 +4336,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="4">
         <v>0.39577169558249597</v>
       </c>
       <c r="B14">
@@ -967,10 +4348,10 @@
       <c r="D14">
         <v>81</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="4">
         <v>0.26733590211979102</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <v>0.72093023117198496</v>
       </c>
       <c r="G14" t="s">
@@ -978,7 +4359,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="4">
         <v>0.233829325427204</v>
       </c>
       <c r="B15">
@@ -990,10 +4371,10 @@
       <c r="D15">
         <v>99</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="4">
         <v>0.27410680228887602</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
         <v>0.69767441721849599</v>
       </c>
       <c r="G15" t="s">
@@ -1001,7 +4382,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="4">
         <v>0.20838181566157901</v>
       </c>
       <c r="B16">
@@ -1013,10 +4394,10 @@
       <c r="D16">
         <v>93</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="4">
         <v>0.29288523557574198</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="3">
         <v>0.69767441721849599</v>
       </c>
       <c r="G16" t="s">
@@ -1024,7 +4405,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="4">
         <v>0.2</v>
       </c>
       <c r="B17">
@@ -1036,10 +4417,10 @@
       <c r="D17">
         <v>120</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="4">
         <v>0.29432293564774198</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="3">
         <v>0.69767441721849599</v>
       </c>
       <c r="G17" t="s">
@@ -1047,7 +4428,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="4">
         <v>0.38423630784907897</v>
       </c>
       <c r="B18">
@@ -1059,10 +4440,10 @@
       <c r="D18">
         <v>95</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="4">
         <v>0.29524493771929999</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="3">
         <v>0.69767441721849599</v>
       </c>
       <c r="G18" t="s">
@@ -1070,7 +4451,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="4">
         <v>0.24786251961875</v>
       </c>
       <c r="B19">
@@ -1082,10 +4463,10 @@
       <c r="D19">
         <v>101</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="4">
         <v>0.310734415470167</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="3">
         <v>0.67441860326500802</v>
       </c>
       <c r="G19" t="s">
@@ -1093,7 +4474,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="4">
         <v>0.42492890731560701</v>
       </c>
       <c r="B20">
@@ -1105,10 +4486,10 @@
       <c r="D20">
         <v>64</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="4">
         <v>0.35588541800199502</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="3">
         <v>0.65116278931151905</v>
       </c>
       <c r="G20" t="s">
@@ -1116,7 +4497,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="4">
         <v>0.219713846911579</v>
       </c>
       <c r="B21">
@@ -1128,10 +4509,10 @@
       <c r="D21">
         <v>149</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="4">
         <v>0.34229188706985703</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="3">
         <v>0.65116278931151905</v>
       </c>
       <c r="G21" t="s">
@@ -1139,7 +4520,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="4">
         <v>0.36497541610466999</v>
       </c>
       <c r="B22">
@@ -1151,10 +4532,10 @@
       <c r="D22">
         <v>124</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="4">
         <v>0.244455299405164</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="3">
         <v>0.60465116833531496</v>
       </c>
       <c r="G22" t="s">
@@ -1162,7 +4543,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="4">
         <v>0.35909773055779498</v>
       </c>
       <c r="B23">
@@ -1174,10 +4555,10 @@
       <c r="D23">
         <v>90</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="4">
         <v>0.255431518998256</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="3">
         <v>0.60465116833531496</v>
       </c>
       <c r="G23" t="s">
@@ -1185,7 +4566,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="A24" s="4">
         <v>0.47818073837029501</v>
       </c>
       <c r="B24">
@@ -1197,10 +4578,10 @@
       <c r="D24">
         <v>99</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="4">
         <v>0.25839080228361899</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="3">
         <v>0.60465116833531496</v>
       </c>
       <c r="G24" t="s">
@@ -1220,10 +4601,10 @@
       <c r="D25">
         <v>138</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="4">
         <v>0.239084055603936</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="3">
         <v>0.60465116001838803</v>
       </c>
       <c r="G25" t="s">
@@ -1235,6 +4616,7 @@
     <sortCondition descending="1" ref="F2:F25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1242,7 +4624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A651DD34-854C-7143-8D50-B2457B0FF092}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modified for PDF printing
</commit_message>
<xml_diff>
--- a/data/Results/SciEntsData Hypertuning.xlsx
+++ b/data/Results/SciEntsData Hypertuning.xlsx
@@ -8,17 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dbrandt/Dropbox/PycharmProjects/short_answer_granding_capstone_project/data/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1063DEF-2AA8-9041-8063-2785BC24D3BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0851E4DF-9B65-F743-83BE-68613F63B27D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26220" yWindow="1400" windowWidth="28040" windowHeight="17440" xr2:uid="{74EE537B-979F-D844-81CC-929D075ED3E5}"/>
+    <workbookView xWindow="26200" yWindow="1400" windowWidth="41160" windowHeight="25100" xr2:uid="{74EE537B-979F-D844-81CC-929D075ED3E5}"/>
   </bookViews>
   <sheets>
     <sheet name="SciEntsData Hypertuning Results" sheetId="1" r:id="rId1"/>
     <sheet name="Source Sentences" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,21 +34,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="83">
   <si>
-    <t>Validation_loss</t>
-  </si>
-  <si>
-    <t>Validation_accuracy</t>
-  </si>
-  <si>
     <t>log</t>
   </si>
   <si>
     <t>dropout</t>
   </si>
   <si>
-    <t>embedding_size</t>
-  </si>
-  <si>
     <t>epochs</t>
   </si>
   <si>
@@ -284,6 +272,15 @@
   </si>
   <si>
     <t>Like poles repel and opposite poles attract.</t>
+  </si>
+  <si>
+    <t>embedding size</t>
+  </si>
+  <si>
+    <t>Validation Loss</t>
+  </si>
+  <si>
+    <t>Validation accuracy</t>
   </si>
 </sst>
 </file>
@@ -292,7 +289,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -343,8 +340,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,6 +649,8 @@
         <c:axId val="1763048527"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.5"/>
+          <c:min val="0.15000000000000002"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -710,6 +713,8 @@
         <c:axId val="1763050159"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.9"/>
+          <c:min val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -879,7 +884,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>embedding_size</c:v>
+                  <c:v>embedding size</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1105,6 +1110,7 @@
         <c:axId val="1763048527"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="110"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1167,6 +1173,8 @@
         <c:axId val="1763050159"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.9"/>
+          <c:min val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1561,6 +1569,8 @@
         <c:axId val="1763048527"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="190"/>
+          <c:min val="55"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1623,6 +1633,7 @@
         <c:axId val="1763050159"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3406,15 +3417,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>838200</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3442,15 +3453,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>863600</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3480,15 +3491,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>825500</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3516,214 +3527,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="ShortAnswer Hypertuning Results"/>
-      <sheetName val="Source Sentences"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="A2">
-            <v>0.38547532152095398</v>
-          </cell>
-          <cell r="F2">
-            <v>0.76744186600973396</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>0.22199686351997999</v>
-          </cell>
-          <cell r="F3">
-            <v>0.76744185907896101</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>0.20300461839595399</v>
-          </cell>
-          <cell r="F4">
-            <v>0.74418605205624599</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>0.38364195774972998</v>
-          </cell>
-          <cell r="F5">
-            <v>0.74418604512547304</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>0.44596580996139501</v>
-          </cell>
-          <cell r="F6">
-            <v>0.74418604512547304</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>0.23362639056012</v>
-          </cell>
-          <cell r="F7">
-            <v>0.74418604512547304</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>0.36786325122251501</v>
-          </cell>
-          <cell r="F8">
-            <v>0.74418604512547304</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>0.39112717698970401</v>
-          </cell>
-          <cell r="F9">
-            <v>0.74418604512547304</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>0.223719950427204</v>
-          </cell>
-          <cell r="F10">
-            <v>0.72093023810275703</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>0.37640549730220402</v>
-          </cell>
-          <cell r="F11">
-            <v>0.72093023117198496</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>0.35601975511470402</v>
-          </cell>
-          <cell r="F12">
-            <v>0.72093023117198496</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>0.20300461839595399</v>
-          </cell>
-          <cell r="F13">
-            <v>0.72093023117198496</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>0.39577169558249597</v>
-          </cell>
-          <cell r="F14">
-            <v>0.72093023117198496</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>0.233829325427204</v>
-          </cell>
-          <cell r="F15">
-            <v>0.69767441721849599</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>0.20838181566157901</v>
-          </cell>
-          <cell r="F16">
-            <v>0.69767441721849599</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>0.2</v>
-          </cell>
-          <cell r="F17">
-            <v>0.69767441721849599</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>0.38423630784907897</v>
-          </cell>
-          <cell r="F18">
-            <v>0.69767441721849599</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>0.24786251961875</v>
-          </cell>
-          <cell r="F19">
-            <v>0.67441860326500802</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>0.42492890731560701</v>
-          </cell>
-          <cell r="F20">
-            <v>0.65116278931151905</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>0.219713846911579</v>
-          </cell>
-          <cell r="F21">
-            <v>0.65116278931151905</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>0.36497541610466999</v>
-          </cell>
-          <cell r="F22">
-            <v>0.60465116833531496</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>0.35909773055779498</v>
-          </cell>
-          <cell r="F23">
-            <v>0.60465116833531496</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>0.47818073837029501</v>
-          </cell>
-          <cell r="F24">
-            <v>0.60465116833531496</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>0.32545903287280598</v>
-          </cell>
-          <cell r="F25">
-            <v>0.60465116001838803</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4025,590 +3828,594 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4187893-C62D-BB41-AE0E-B9FEF22E5CB0}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="60" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="17" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="60" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>0.38547532152095398</v>
+      </c>
+      <c r="B2" s="2">
+        <v>52</v>
+      </c>
+      <c r="C2" s="2">
+        <v>200</v>
+      </c>
+      <c r="D2" s="2">
+        <v>147</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.255741164434787</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.76744186600973396</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>0.22199686351997999</v>
+      </c>
+      <c r="B3" s="2">
+        <v>54</v>
+      </c>
+      <c r="C3" s="2">
+        <v>200</v>
+      </c>
+      <c r="D3" s="2">
+        <v>97</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.24057497915833401</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0.76744185907896101</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>0.20300461839595399</v>
+      </c>
+      <c r="B4" s="2">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2">
+        <v>200</v>
+      </c>
+      <c r="D4" s="2">
+        <v>118</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.26060245480648297</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.74418605205624599</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>0.38364195774972998</v>
+      </c>
+      <c r="B5" s="2">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2">
+        <v>222</v>
+      </c>
+      <c r="D5" s="2">
+        <v>179</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.27446782138458498</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.74418604512547304</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>0.44596580996139501</v>
+      </c>
+      <c r="B6" s="2">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2">
+        <v>164</v>
+      </c>
+      <c r="D6" s="2">
+        <v>83</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.24562144314133799</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.74418604512547304</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>0.23362639056012</v>
+      </c>
+      <c r="B7" s="2">
+        <v>68</v>
+      </c>
+      <c r="C7" s="2">
+        <v>200</v>
+      </c>
+      <c r="D7" s="2">
+        <v>107</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.24299895936666499</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.74418604512547304</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>0.36786325122251501</v>
+      </c>
+      <c r="B8" s="2">
+        <v>87</v>
+      </c>
+      <c r="C8" s="2">
+        <v>200</v>
+      </c>
+      <c r="D8" s="2">
+        <v>124</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.24509148403655601</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.74418604512547304</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>0.39112717698970401</v>
+      </c>
+      <c r="B9" s="2">
+        <v>46</v>
+      </c>
+      <c r="C9" s="2">
+        <v>200</v>
+      </c>
+      <c r="D9" s="2">
+        <v>93</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.279094595202179</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.74418604512547304</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>0.223719950427204</v>
+      </c>
+      <c r="B10" s="2">
+        <v>92</v>
+      </c>
+      <c r="C10" s="2">
+        <v>200</v>
+      </c>
+      <c r="D10" s="2">
+        <v>88</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.28327261050080099</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.72093023810275703</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>0.37640549730220402</v>
+      </c>
+      <c r="B11" s="2">
+        <v>94</v>
+      </c>
+      <c r="C11" s="2">
+        <v>200</v>
+      </c>
+      <c r="D11" s="2">
+        <v>133</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.30613542053588599</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.72093023117198496</v>
+      </c>
+      <c r="G11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>0.35601975511470402</v>
+      </c>
+      <c r="B12" s="2">
+        <v>68</v>
+      </c>
+      <c r="C12" s="2">
+        <v>200</v>
+      </c>
+      <c r="D12" s="2">
+        <v>108</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.27214143373245397</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.72093023117198496</v>
+      </c>
+      <c r="G12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>0.20300461839595399</v>
+      </c>
+      <c r="B13" s="2">
+        <v>41</v>
+      </c>
+      <c r="C13" s="2">
+        <v>200</v>
+      </c>
+      <c r="D13" s="2">
+        <v>119</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.27320282785005301</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.72093023117198496</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>0.39577169558249597</v>
+      </c>
+      <c r="B14" s="2">
+        <v>66</v>
+      </c>
+      <c r="C14" s="2">
+        <v>200</v>
+      </c>
+      <c r="D14" s="2">
+        <v>81</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.26733590211979102</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.72093023117198496</v>
+      </c>
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>0.233829325427204</v>
+      </c>
+      <c r="B15" s="2">
+        <v>51</v>
+      </c>
+      <c r="C15" s="2">
+        <v>200</v>
+      </c>
+      <c r="D15" s="2">
+        <v>99</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.27410680228887602</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.69767441721849599</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>0.20838181566157901</v>
+      </c>
+      <c r="B16" s="2">
+        <v>100</v>
+      </c>
+      <c r="C16" s="2">
+        <v>200</v>
+      </c>
+      <c r="D16" s="2">
+        <v>93</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.29288523557574198</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.69767441721849599</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="B17" s="2">
+        <v>39</v>
+      </c>
+      <c r="C17" s="2">
+        <v>200</v>
+      </c>
+      <c r="D17" s="2">
+        <v>120</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.29432293564774198</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0.69767441721849599</v>
+      </c>
+      <c r="G17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>0.38423630784907897</v>
+      </c>
+      <c r="B18" s="2">
+        <v>58</v>
+      </c>
+      <c r="C18" s="2">
+        <v>200</v>
+      </c>
+      <c r="D18" s="2">
+        <v>95</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.29524493771929999</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.69767441721849599</v>
+      </c>
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>0.24786251961875</v>
+      </c>
+      <c r="B19" s="2">
+        <v>76</v>
+      </c>
+      <c r="C19" s="2">
+        <v>200</v>
+      </c>
+      <c r="D19" s="2">
+        <v>101</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.310734415470167</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.67441860326500802</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>0.42492890731560701</v>
+      </c>
+      <c r="B20" s="2">
+        <v>63</v>
+      </c>
+      <c r="C20" s="2">
+        <v>192</v>
+      </c>
+      <c r="D20" s="2">
+        <v>64</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.35588541800199502</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.65116278931151905</v>
+      </c>
+      <c r="G20" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="4">
-        <v>0.38547532152095398</v>
-      </c>
-      <c r="B2">
-        <v>52</v>
-      </c>
-      <c r="C2">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>0.219713846911579</v>
+      </c>
+      <c r="B21" s="2">
+        <v>81</v>
+      </c>
+      <c r="C21" s="2">
         <v>200</v>
       </c>
-      <c r="D2">
-        <v>147</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0.255741164434787</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0.76744186600973396</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="D21" s="2">
+        <v>149</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.34229188706985703</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.65116278931151905</v>
+      </c>
+      <c r="G21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
-        <v>0.22199686351997999</v>
-      </c>
-      <c r="B3">
-        <v>54</v>
-      </c>
-      <c r="C3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>0.36497541610466999</v>
+      </c>
+      <c r="B22" s="2">
+        <v>10</v>
+      </c>
+      <c r="C22" s="2">
+        <v>133</v>
+      </c>
+      <c r="D22" s="2">
+        <v>124</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.244455299405164</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.60465116833531496</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>0.35909773055779498</v>
+      </c>
+      <c r="B23" s="2">
+        <v>13</v>
+      </c>
+      <c r="C23" s="2">
+        <v>115</v>
+      </c>
+      <c r="D23" s="2">
+        <v>90</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.255431518998256</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0.60465116833531496</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>0.47818073837029501</v>
+      </c>
+      <c r="B24" s="2">
+        <v>10</v>
+      </c>
+      <c r="C24" s="2">
+        <v>95</v>
+      </c>
+      <c r="D24" s="2">
+        <v>99</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.25839080228361899</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0.60465116833531496</v>
+      </c>
+      <c r="G24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>0.32545903287280598</v>
+      </c>
+      <c r="B25" s="2">
+        <v>85</v>
+      </c>
+      <c r="C25" s="2">
         <v>200</v>
       </c>
-      <c r="D3">
-        <v>97</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.24057497915833401</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.76744185907896101</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
-        <v>0.20300461839595399</v>
-      </c>
-      <c r="B4">
-        <v>39</v>
-      </c>
-      <c r="C4">
-        <v>200</v>
-      </c>
-      <c r="D4">
-        <v>118</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.26060245480648297</v>
-      </c>
-      <c r="F4" s="3">
-        <v>0.74418605205624599</v>
-      </c>
-      <c r="G4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
-        <v>0.38364195774972998</v>
-      </c>
-      <c r="B5">
-        <v>23</v>
-      </c>
-      <c r="C5">
-        <v>222</v>
-      </c>
-      <c r="D5">
-        <v>179</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.27446782138458498</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.74418604512547304</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <v>0.44596580996139501</v>
-      </c>
-      <c r="B6">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>164</v>
-      </c>
-      <c r="D6">
-        <v>83</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.24562144314133799</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.74418604512547304</v>
-      </c>
-      <c r="G6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
-        <v>0.23362639056012</v>
-      </c>
-      <c r="B7">
-        <v>68</v>
-      </c>
-      <c r="C7">
-        <v>200</v>
-      </c>
-      <c r="D7">
-        <v>107</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.24299895936666499</v>
-      </c>
-      <c r="F7" s="3">
-        <v>0.74418604512547304</v>
-      </c>
-      <c r="G7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
-        <v>0.36786325122251501</v>
-      </c>
-      <c r="B8">
-        <v>87</v>
-      </c>
-      <c r="C8">
-        <v>200</v>
-      </c>
-      <c r="D8">
-        <v>124</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.24509148403655601</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.74418604512547304</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
-        <v>0.39112717698970401</v>
-      </c>
-      <c r="B9">
-        <v>46</v>
-      </c>
-      <c r="C9">
-        <v>200</v>
-      </c>
-      <c r="D9">
-        <v>93</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0.279094595202179</v>
-      </c>
-      <c r="F9" s="3">
-        <v>0.74418604512547304</v>
-      </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
-        <v>0.223719950427204</v>
-      </c>
-      <c r="B10">
-        <v>92</v>
-      </c>
-      <c r="C10">
-        <v>200</v>
-      </c>
-      <c r="D10">
-        <v>88</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.28327261050080099</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0.72093023810275703</v>
-      </c>
-      <c r="G10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
-        <v>0.37640549730220402</v>
-      </c>
-      <c r="B11">
-        <v>94</v>
-      </c>
-      <c r="C11">
-        <v>200</v>
-      </c>
-      <c r="D11">
-        <v>133</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0.30613542053588599</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0.72093023117198496</v>
-      </c>
-      <c r="G11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="4">
-        <v>0.35601975511470402</v>
-      </c>
-      <c r="B12">
-        <v>68</v>
-      </c>
-      <c r="C12">
-        <v>200</v>
-      </c>
-      <c r="D12">
-        <v>108</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0.27214143373245397</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0.72093023117198496</v>
-      </c>
-      <c r="G12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="4">
-        <v>0.20300461839595399</v>
-      </c>
-      <c r="B13">
-        <v>41</v>
-      </c>
-      <c r="C13">
-        <v>200</v>
-      </c>
-      <c r="D13">
-        <v>119</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0.27320282785005301</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0.72093023117198496</v>
-      </c>
-      <c r="G13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="4">
-        <v>0.39577169558249597</v>
-      </c>
-      <c r="B14">
-        <v>66</v>
-      </c>
-      <c r="C14">
-        <v>200</v>
-      </c>
-      <c r="D14">
-        <v>81</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0.26733590211979102</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.72093023117198496</v>
-      </c>
-      <c r="G14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
-        <v>0.233829325427204</v>
-      </c>
-      <c r="B15">
-        <v>51</v>
-      </c>
-      <c r="C15">
-        <v>200</v>
-      </c>
-      <c r="D15">
-        <v>99</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0.27410680228887602</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.69767441721849599</v>
-      </c>
-      <c r="G15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
-        <v>0.20838181566157901</v>
-      </c>
-      <c r="B16">
-        <v>100</v>
-      </c>
-      <c r="C16">
-        <v>200</v>
-      </c>
-      <c r="D16">
-        <v>93</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0.29288523557574198</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0.69767441721849599</v>
-      </c>
-      <c r="G16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="B17">
-        <v>39</v>
-      </c>
-      <c r="C17">
-        <v>200</v>
-      </c>
-      <c r="D17">
-        <v>120</v>
-      </c>
-      <c r="E17" s="4">
-        <v>0.29432293564774198</v>
-      </c>
-      <c r="F17" s="3">
-        <v>0.69767441721849599</v>
-      </c>
-      <c r="G17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
-        <v>0.38423630784907897</v>
-      </c>
-      <c r="B18">
-        <v>58</v>
-      </c>
-      <c r="C18">
-        <v>200</v>
-      </c>
-      <c r="D18">
-        <v>95</v>
-      </c>
-      <c r="E18" s="4">
-        <v>0.29524493771929999</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.69767441721849599</v>
-      </c>
-      <c r="G18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="4">
-        <v>0.24786251961875</v>
-      </c>
-      <c r="B19">
-        <v>76</v>
-      </c>
-      <c r="C19">
-        <v>200</v>
-      </c>
-      <c r="D19">
-        <v>101</v>
-      </c>
-      <c r="E19" s="4">
-        <v>0.310734415470167</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0.67441860326500802</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="D25" s="2">
+        <v>138</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.239084055603936</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0.60465116001838803</v>
+      </c>
+      <c r="G25" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="4">
-        <v>0.42492890731560701</v>
-      </c>
-      <c r="B20">
-        <v>63</v>
-      </c>
-      <c r="C20">
-        <v>192</v>
-      </c>
-      <c r="D20">
-        <v>64</v>
-      </c>
-      <c r="E20" s="4">
-        <v>0.35588541800199502</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0.65116278931151905</v>
-      </c>
-      <c r="G20" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="4">
-        <v>0.219713846911579</v>
-      </c>
-      <c r="B21">
-        <v>81</v>
-      </c>
-      <c r="C21">
-        <v>200</v>
-      </c>
-      <c r="D21">
-        <v>149</v>
-      </c>
-      <c r="E21" s="4">
-        <v>0.34229188706985703</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0.65116278931151905</v>
-      </c>
-      <c r="G21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="4">
-        <v>0.36497541610466999</v>
-      </c>
-      <c r="B22">
-        <v>10</v>
-      </c>
-      <c r="C22">
-        <v>133</v>
-      </c>
-      <c r="D22">
-        <v>124</v>
-      </c>
-      <c r="E22" s="4">
-        <v>0.244455299405164</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0.60465116833531496</v>
-      </c>
-      <c r="G22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
-        <v>0.35909773055779498</v>
-      </c>
-      <c r="B23">
-        <v>13</v>
-      </c>
-      <c r="C23">
-        <v>115</v>
-      </c>
-      <c r="D23">
-        <v>90</v>
-      </c>
-      <c r="E23" s="4">
-        <v>0.255431518998256</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0.60465116833531496</v>
-      </c>
-      <c r="G23" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
-        <v>0.47818073837029501</v>
-      </c>
-      <c r="B24">
-        <v>10</v>
-      </c>
-      <c r="C24">
-        <v>95</v>
-      </c>
-      <c r="D24">
-        <v>99</v>
-      </c>
-      <c r="E24" s="4">
-        <v>0.25839080228361899</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0.60465116833531496</v>
-      </c>
-      <c r="G24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>0.32545903287280598</v>
-      </c>
-      <c r="B25">
-        <v>85</v>
-      </c>
-      <c r="C25">
-        <v>200</v>
-      </c>
-      <c r="D25">
-        <v>138</v>
-      </c>
-      <c r="E25" s="4">
-        <v>0.239084055603936</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0.60465116001838803</v>
-      </c>
-      <c r="G25" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -4616,6 +4423,7 @@
     <sortCondition descending="1" ref="F2:F25"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -4638,13 +4446,13 @@
     <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -4665,7 +4473,7 @@
         <v xml:space="preserve"> the nickel is the hardest becaus is you scratch it with a penni it will not scratch but the nickel could becaus it is so much</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G2">
         <f>H2+1</f>
@@ -4675,13 +4483,13 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -4702,7 +4510,7 @@
         <v xml:space="preserve"> which had less scratch</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G43" si="1">H3+1</f>
@@ -4712,13 +4520,13 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -4739,7 +4547,7 @@
         <v xml:space="preserve"> how you would know that one of them is harder is for say if the nickel never a scratch the penni and the penni got scratch by the nickel then the nickel would be harder than the penni that is how you would which one is harder</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
@@ -4749,13 +4557,13 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -4776,7 +4584,7 @@
         <v xml:space="preserve"> when it wa loos the sound wa soft but when it wa tighten it is low</v>
       </c>
       <c r="F5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
@@ -4786,13 +4594,13 @@
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -4813,7 +4621,7 @@
         <v xml:space="preserve"> the ring do not touch becaus the ring are just magnet and the magnet are on the repel side</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
@@ -4823,13 +4631,13 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -4850,7 +4658,7 @@
         <v xml:space="preserve"> in order to tell which is harder els would have to see if the penni and nickel leav a mark to see which is harder</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
@@ -4860,13 +4668,13 @@
         <v>5</v>
       </c>
       <c r="I7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -4887,7 +4695,7 @@
         <v xml:space="preserve"> they do not touch each other becaus if you put magnet the magnet like thi will not attract north to north if you put magnet like thi it will attract north to south if you put it like thi it will not attract south to south</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
@@ -4897,13 +4705,13 @@
         <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -4924,7 +4732,7 @@
         <v xml:space="preserve"> it would make a high sound</v>
       </c>
       <c r="F9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
@@ -4934,13 +4742,13 @@
         <v>7</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -4961,7 +4769,7 @@
         <v xml:space="preserve"> a solut is when you take a mixtur like powder and mix it with water then after stir it it becom a solut</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
@@ -4971,13 +4779,13 @@
         <v>8</v>
       </c>
       <c r="I10" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -4998,7 +4806,7 @@
         <v xml:space="preserve"> in a solut one of the materi dissolv and the mixtur is see through</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
@@ -5008,13 +4816,13 @@
         <v>9</v>
       </c>
       <c r="I11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -5026,13 +4834,13 @@
         <v>10</v>
       </c>
       <c r="I12" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -5044,13 +4852,13 @@
         <v>11</v>
       </c>
       <c r="I13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -5062,13 +4870,13 @@
         <v>12</v>
       </c>
       <c r="I14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -5080,13 +4888,13 @@
         <v>13</v>
       </c>
       <c r="I15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -5098,13 +4906,13 @@
         <v>14</v>
       </c>
       <c r="I16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="7:11" x14ac:dyDescent="0.2">
@@ -5116,13 +4924,13 @@
         <v>15</v>
       </c>
       <c r="I17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J17" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="7:11" x14ac:dyDescent="0.2">
@@ -5134,13 +4942,13 @@
         <v>16</v>
       </c>
       <c r="I18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J18" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="7:11" x14ac:dyDescent="0.2">
@@ -5152,13 +4960,13 @@
         <v>17</v>
       </c>
       <c r="I19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="7:11" x14ac:dyDescent="0.2">
@@ -5170,13 +4978,13 @@
         <v>18</v>
       </c>
       <c r="I20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="7:11" x14ac:dyDescent="0.2">
@@ -5188,13 +4996,13 @@
         <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="7:11" x14ac:dyDescent="0.2">
@@ -5206,13 +5014,13 @@
         <v>20</v>
       </c>
       <c r="I22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J22" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="7:11" x14ac:dyDescent="0.2">
@@ -5224,13 +5032,13 @@
         <v>21</v>
       </c>
       <c r="I23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K23" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="7:11" x14ac:dyDescent="0.2">
@@ -5242,13 +5050,13 @@
         <v>22</v>
       </c>
       <c r="I24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K24" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="7:11" x14ac:dyDescent="0.2">
@@ -5260,13 +5068,13 @@
         <v>23</v>
       </c>
       <c r="I25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K25" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="7:11" x14ac:dyDescent="0.2">
@@ -5278,13 +5086,13 @@
         <v>24</v>
       </c>
       <c r="I26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="7:11" x14ac:dyDescent="0.2">
@@ -5296,13 +5104,13 @@
         <v>25</v>
       </c>
       <c r="I27" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K27" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="7:11" x14ac:dyDescent="0.2">
@@ -5314,13 +5122,13 @@
         <v>26</v>
       </c>
       <c r="I28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J28" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="7:11" x14ac:dyDescent="0.2">
@@ -5332,13 +5140,13 @@
         <v>27</v>
       </c>
       <c r="I29" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J29" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K29" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="7:11" x14ac:dyDescent="0.2">
@@ -5350,13 +5158,13 @@
         <v>28</v>
       </c>
       <c r="I30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J30" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="7:11" x14ac:dyDescent="0.2">
@@ -5368,13 +5176,13 @@
         <v>29</v>
       </c>
       <c r="I31" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="7:11" x14ac:dyDescent="0.2">
@@ -5386,13 +5194,13 @@
         <v>30</v>
       </c>
       <c r="I32" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K32" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="7:11" x14ac:dyDescent="0.2">
@@ -5404,13 +5212,13 @@
         <v>31</v>
       </c>
       <c r="I33" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J33" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K33" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="7:11" x14ac:dyDescent="0.2">
@@ -5422,13 +5230,13 @@
         <v>32</v>
       </c>
       <c r="I34" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="7:11" x14ac:dyDescent="0.2">
@@ -5440,13 +5248,13 @@
         <v>33</v>
       </c>
       <c r="I35" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K35" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="7:11" x14ac:dyDescent="0.2">
@@ -5458,13 +5266,13 @@
         <v>34</v>
       </c>
       <c r="I36" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J36" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K36" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="7:11" x14ac:dyDescent="0.2">
@@ -5476,13 +5284,13 @@
         <v>35</v>
       </c>
       <c r="I37" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J37" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K37" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="7:11" x14ac:dyDescent="0.2">
@@ -5494,13 +5302,13 @@
         <v>36</v>
       </c>
       <c r="I38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J38" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K38" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="7:11" x14ac:dyDescent="0.2">
@@ -5512,13 +5320,13 @@
         <v>37</v>
       </c>
       <c r="I39" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J39" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K39" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="7:11" x14ac:dyDescent="0.2">
@@ -5530,13 +5338,13 @@
         <v>38</v>
       </c>
       <c r="I40" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J40" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K40" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="7:11" x14ac:dyDescent="0.2">
@@ -5548,13 +5356,13 @@
         <v>39</v>
       </c>
       <c r="I41" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J41" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K41" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="7:11" x14ac:dyDescent="0.2">
@@ -5566,13 +5374,13 @@
         <v>40</v>
       </c>
       <c r="I42" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J42" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K42" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="7:11" x14ac:dyDescent="0.2">
@@ -5584,16 +5392,17 @@
         <v>41</v>
       </c>
       <c r="I43" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J43" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K43" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>